<commit_message>
new update to location
</commit_message>
<xml_diff>
--- a/SF_golden_retrievers_notes_docs.xlsx
+++ b/SF_golden_retrievers_notes_docs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kobetran/Documents/Personal_Projects/WebDevelopment/puppystore_folder/sf-golden-retrievers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124BAAEB-26DC-4E4E-ABED-2255BF6E513B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE807CDA-3864-064C-B49D-004F4D8D9D76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22720" yWindow="4400" windowWidth="28100" windowHeight="17440" xr2:uid="{EF9E5897-A4C8-0940-835F-E98CCC07B42F}"/>
+    <workbookView xWindow="22720" yWindow="4400" windowWidth="28100" windowHeight="17440" activeTab="1" xr2:uid="{EF9E5897-A4C8-0940-835F-E98CCC07B42F}"/>
   </bookViews>
   <sheets>
     <sheet name="SF Golden Retrievers Docs" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>https://www.youtube.com/watch?v=zxfhf-V4JFQ</t>
   </si>
@@ -51,6 +52,9 @@
   </si>
   <si>
     <t>trying to reuse nav bar throughout all pages</t>
+  </si>
+  <si>
+    <t>Need to add nav button</t>
   </si>
 </sst>
 </file>
@@ -418,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0931B72C-E13B-174B-82B7-F0BD30C5A385}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -459,4 +463,22 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1030E9BE-D40B-AC40-B2F5-908DDC0CE9D8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>